<commit_message>
Updated data.html and data files
</commit_message>
<xml_diff>
--- a/docs/Data/Grades_L3_hw_quiz.xlsx
+++ b/docs/Data/Grades_L3_hw_quiz.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webmailbyui-my.sharepoint.com/personal/drp36_byui_edu/Documents/221/Course_Files/BYUI_M221_Book/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Downloads\Temp data folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D423FA-9B5A-417B-88A6-2BDEFE78DFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,13 +35,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Grade</t>
+    <t>grade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -385,116 +386,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>65</v>
       </c>
@@ -506,6 +505,66 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FolderType xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <Owner xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Students xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Student_Groups xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <TeamsChannelId xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <NotebookType xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <Distribution_Groups xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <Math_Settings xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <Invited_Teachers xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <Invited_Students xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <Templates xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <Teachers xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <AppVersion xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <CultureName xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+    <LMS_Mappings xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000FFD864706841F429944AA8AEC96A5F6" ma:contentTypeVersion="35" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="58019298a95b80a072b42d332cb397db">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="56caf978-ed08-4319-8660-ea565c3c81d4" xmlns:ns4="1c0769b7-2dc5-4346-9277-bf71cefdc793" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="92a71820afc3cddf950a71f89fd1abfc" ns3:_="" ns4:_="">
     <xsd:import namespace="56caf978-ed08-4319-8660-ea565c3c81d4"/>
@@ -930,67 +989,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F98267CA-32BF-4FA9-9D2B-1D35444314D2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1c0769b7-2dc5-4346-9277-bf71cefdc793"/>
+    <ds:schemaRef ds:uri="56caf978-ed08-4319-8660-ea565c3c81d4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FolderType xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <Owner xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Students xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Student_Groups xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <TeamsChannelId xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <NotebookType xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <Distribution_Groups xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <Math_Settings xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <Invited_Teachers xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <Invited_Students xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <Templates xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <Teachers xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <AppVersion xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <CultureName xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-    <LMS_Mappings xmlns="1c0769b7-2dc5-4346-9277-bf71cefdc793" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EB9ABD4-8097-4089-82BA-71123B5AE879}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8265420C-9319-4291-8207-59E18FACDA67}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1007,29 +1031,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EB9ABD4-8097-4089-82BA-71123B5AE879}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F98267CA-32BF-4FA9-9D2B-1D35444314D2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1c0769b7-2dc5-4346-9277-bf71cefdc793"/>
-    <ds:schemaRef ds:uri="56caf978-ed08-4319-8660-ea565c3c81d4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>